<commit_message>
backend audit file generation
</commit_message>
<xml_diff>
--- a/backend/Book1.xlsx
+++ b/backend/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Epcorn\OneDrive\Desktop\MCD\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85116A1-6DD5-4E2A-B28A-E8293F4EDDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB77863B-BE00-4001-8414-E0A3E132AE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AD6F44CD-47C1-492C-B843-3386E53A42FC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <r>
       <rPr>
@@ -43,55 +43,6 @@
       </rPr>
       <t>Food Leftover</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Oil Residue</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Cracks</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Entrance Door</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Rare Door</t>
-    </r>
-  </si>
-  <si>
-    <t>working</t>
-  </si>
-  <si>
-    <t>Trap Sheet Needs To Replace - No</t>
-  </si>
-  <si>
-    <t>Found Full</t>
   </si>
   <si>
     <t>Name</t>
@@ -130,7 +81,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve">                Date :13/09/2022</t>
+      <t xml:space="preserve">               </t>
     </r>
   </si>
 </sst>
@@ -278,11 +229,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -657,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE35908F-B6EF-47A9-B481-7EB061C72DCF}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,33 +631,33 @@
       <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
-        <v>14</v>
+      <c r="A2" s="7" t="s">
+        <v>7</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -720,25 +671,15 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -746,9 +687,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A7" s="4"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -756,9 +695,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -766,9 +703,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -776,9 +711,7 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A10" s="4"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -786,9 +719,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A11" s="4"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -796,9 +727,7 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A12" s="4"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -806,9 +735,7 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A13" s="4"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>

</xml_diff>